<commit_message>
added various recent changes
</commit_message>
<xml_diff>
--- a/inst/extdata/wms_sources.xlsx
+++ b/inst/extdata/wms_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\PROJEKT\R\eagles\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\projects\R\eagles\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6CE6C2-065F-4BBD-B918-76E5F6F90CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3032D75F-A9F9-4EE6-B1B8-34C538ACBF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9ED8486B-B65A-4296-8AB7-5F597AE3FF3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9ED8486B-B65A-4296-8AB7-5F597AE3FF3F}"/>
   </bookViews>
   <sheets>
     <sheet name="wms_layers" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +435,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -476,6 +483,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -793,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D52AA1-ABAD-4567-88E1-C2B20543F75F}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1668,9 +1676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7B8A3F-FE11-4099-9BDA-704F27868698}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1776,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1776,7 +1784,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B13" s="5" t="s">

</xml_diff>